<commit_message>
latest backup from TBGPEA
</commit_message>
<xml_diff>
--- a/Resolution_scaling_table.xlsx
+++ b/Resolution_scaling_table.xlsx
@@ -9,13 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18384" windowHeight="7872"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18390" windowHeight="7875"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -378,15 +377,15 @@
   <dimension ref="A1:W16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -418,7 +417,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -465,7 +464,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>12</v>
       </c>
@@ -525,7 +524,7 @@
       <c r="V4" s="2"/>
       <c r="W4" s="2"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>11</v>
       </c>
@@ -585,7 +584,7 @@
       <c r="V5" s="2"/>
       <c r="W5" s="2"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>10</v>
       </c>
@@ -645,7 +644,7 @@
       <c r="V6" s="4"/>
       <c r="W6" s="4"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>9</v>
       </c>
@@ -709,7 +708,7 @@
       <c r="V7" s="4"/>
       <c r="W7" s="4"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>8</v>
       </c>
@@ -773,7 +772,7 @@
       <c r="V8" s="4"/>
       <c r="W8" s="4"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -837,7 +836,7 @@
       <c r="V9" s="4"/>
       <c r="W9" s="4"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -901,7 +900,7 @@
       <c r="V10" s="4"/>
       <c r="W10" s="4"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>
@@ -965,7 +964,7 @@
       <c r="V11" s="4"/>
       <c r="W11" s="4"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
@@ -1029,7 +1028,7 @@
       <c r="V12" s="4"/>
       <c r="W12" s="4"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>3</v>
       </c>
@@ -1093,7 +1092,7 @@
       <c r="V13" s="4"/>
       <c r="W13" s="4"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
@@ -1157,7 +1156,7 @@
       <c r="V14" s="6"/>
       <c r="W14" s="6"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1181,14 +1180,14 @@
         <v>1.6</v>
       </c>
       <c r="H15" s="4"/>
-      <c r="I15" s="5">
+      <c r="I15" s="4">
         <v>1</v>
       </c>
-      <c r="J15" s="5">
+      <c r="J15" s="4">
         <f t="shared" si="4"/>
         <v>32</v>
       </c>
-      <c r="K15" s="5">
+      <c r="K15" s="4">
         <f t="shared" si="5"/>
         <v>3.2</v>
       </c>
@@ -1221,7 +1220,7 @@
       <c r="V15" s="4"/>
       <c r="W15" s="4"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>

</xml_diff>